<commit_message>
arranging the image letter A
</commit_message>
<xml_diff>
--- a/informacoes_nfe.xlsx
+++ b/informacoes_nfe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Hdlogika\k\Backup_19_08_2021\Unidade_D\K\LEATICIA\Luiz Fernando\NFE_Automation\NFE_Logika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6086497D-ABA1-457F-A7F8-F17381008E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9515D682-BE48-458F-ADB9-C677D79F3FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1264,7 +1264,7 @@
   <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>